<commit_message>
V 1.0.1 Dyeminish changes- fixed formatting, now detects DyeTect cases
</commit_message>
<xml_diff>
--- a/Dyeminish-template.xlsx
+++ b/Dyeminish-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zpedersen\ReportProject\ReportGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3074F8E0-6A46-440F-9B27-5DEDA9B731FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41E04EC-B86E-434A-A1DD-93DBCE030FD9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-2310" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F173" sheetId="6" r:id="rId1"/>
@@ -95,7 +95,7 @@
     <t>Percent of threhold with theoretical value</t>
   </si>
   <si>
-    <t>Theoretical volume if dyvert was on continuously (mL)</t>
+    <t>Theoretical cummulative volume to patient if DyeVert was on continuously (mL)</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed Dyeminish injection data
</commit_message>
<xml_diff>
--- a/Dyeminish-template.xlsx
+++ b/Dyeminish-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zpedersen\PycharmProjects\ReportGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A745A36C-65F8-46EC-A0A3-8C2A9EE838F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CB5559-3BAA-4BE0-8706-23E35DE75AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-6630" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F173" sheetId="6" r:id="rId1"/>
@@ -843,10 +843,10 @@
   </sheetPr>
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="AL10" sqref="AL10"/>
+      <selection pane="bottomLeft" activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1020,7 @@
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="13" t="e">
-        <f>2/I2</f>
+        <f>S2/I2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V2" s="6"/>
@@ -1091,7 +1091,7 @@
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="13" t="e">
-        <f t="shared" ref="U3:U66" si="8">2/I3</f>
+        <f t="shared" ref="U3:U66" si="8">S3/I3</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V3" s="6"/>
@@ -5635,7 +5635,7 @@
       <c r="S67" s="6"/>
       <c r="T67" s="6"/>
       <c r="U67" s="13" t="e">
-        <f t="shared" ref="U67:U130" si="19">2/I67</f>
+        <f t="shared" ref="U67:U130" si="19">S67/I67</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V67" s="6"/>
@@ -10179,7 +10179,7 @@
       <c r="S131" s="6"/>
       <c r="T131" s="6"/>
       <c r="U131" s="13" t="e">
-        <f t="shared" ref="U131:U194" si="30">2/I131</f>
+        <f t="shared" ref="U131:U194" si="30">S131/I131</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V131" s="6"/>
@@ -14723,7 +14723,7 @@
       <c r="S195" s="6"/>
       <c r="T195" s="6"/>
       <c r="U195" s="13" t="e">
-        <f t="shared" ref="U195:U258" si="41">2/I195</f>
+        <f t="shared" ref="U195:U258" si="41">S195/I195</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V195" s="6"/>
@@ -19267,7 +19267,7 @@
       <c r="S259" s="6"/>
       <c r="T259" s="6"/>
       <c r="U259" s="13" t="e">
-        <f t="shared" ref="U259:U322" si="52">2/I259</f>
+        <f t="shared" ref="U259:U322" si="52">S259/I259</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V259" s="6"/>
@@ -23811,7 +23811,7 @@
       <c r="S323" s="6"/>
       <c r="T323" s="6"/>
       <c r="U323" s="13" t="e">
-        <f t="shared" ref="U323:U386" si="63">2/I323</f>
+        <f t="shared" ref="U323:U386" si="63">S323/I323</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V323" s="6"/>
@@ -28355,7 +28355,7 @@
       <c r="S387" s="6"/>
       <c r="T387" s="6"/>
       <c r="U387" s="13" t="e">
-        <f t="shared" ref="U387:U450" si="74">2/I387</f>
+        <f t="shared" ref="U387:U450" si="74">S387/I387</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V387" s="6"/>
@@ -32899,7 +32899,7 @@
       <c r="S451" s="6"/>
       <c r="T451" s="6"/>
       <c r="U451" s="13" t="e">
-        <f t="shared" ref="U451:U514" si="85">2/I451</f>
+        <f t="shared" ref="U451:U514" si="85">S451/I451</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V451" s="6"/>
@@ -37443,7 +37443,7 @@
       <c r="S515" s="6"/>
       <c r="T515" s="6"/>
       <c r="U515" s="13" t="e">
-        <f t="shared" ref="U515:U578" si="96">2/I515</f>
+        <f t="shared" ref="U515:U578" si="96">S515/I515</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V515" s="6"/>
@@ -41987,7 +41987,7 @@
       <c r="S579" s="6"/>
       <c r="T579" s="6"/>
       <c r="U579" s="13" t="e">
-        <f t="shared" ref="U579:U642" si="107">2/I579</f>
+        <f t="shared" ref="U579:U642" si="107">S579/I579</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V579" s="6"/>
@@ -46531,7 +46531,7 @@
       <c r="S643" s="6"/>
       <c r="T643" s="6"/>
       <c r="U643" s="13" t="e">
-        <f t="shared" ref="U643:U706" si="118">2/I643</f>
+        <f t="shared" ref="U643:U706" si="118">S643/I643</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V643" s="6"/>
@@ -51075,7 +51075,7 @@
       <c r="S707" s="6"/>
       <c r="T707" s="6"/>
       <c r="U707" s="13" t="e">
-        <f t="shared" ref="U707:U770" si="129">2/I707</f>
+        <f t="shared" ref="U707:U770" si="129">S707/I707</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V707" s="6"/>
@@ -55619,7 +55619,7 @@
       <c r="S771" s="6"/>
       <c r="T771" s="6"/>
       <c r="U771" s="13" t="e">
-        <f t="shared" ref="U771:U834" si="140">2/I771</f>
+        <f t="shared" ref="U771:U834" si="140">S771/I771</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V771" s="6"/>
@@ -60163,7 +60163,7 @@
       <c r="S835" s="6"/>
       <c r="T835" s="6"/>
       <c r="U835" s="13" t="e">
-        <f t="shared" ref="U835:U898" si="151">2/I835</f>
+        <f t="shared" ref="U835:U898" si="151">S835/I835</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V835" s="6"/>
@@ -64707,7 +64707,7 @@
       <c r="S899" s="6"/>
       <c r="T899" s="6"/>
       <c r="U899" s="13" t="e">
-        <f t="shared" ref="U899:U962" si="162">2/I899</f>
+        <f t="shared" ref="U899:U962" si="162">S899/I899</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V899" s="6"/>
@@ -69251,7 +69251,7 @@
       <c r="S963" s="6"/>
       <c r="T963" s="6"/>
       <c r="U963" s="13" t="e">
-        <f t="shared" ref="U963:U1000" si="173">2/I963</f>
+        <f t="shared" ref="U963:U1000" si="173">S963/I963</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V963" s="6"/>

</xml_diff>

<commit_message>
[RG-14] added counting for cases by month/quarter and added a new sheet to hold that info
</commit_message>
<xml_diff>
--- a/Dyeminish-template.xlsx
+++ b/Dyeminish-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zpedersen\PycharmProjects\ReportGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15779AD-C8CE-4266-A62A-61F34AE5DD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5215DF91-EBBC-4A31-B1A3-7E97EC35FDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4620" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F173" sheetId="6" r:id="rId1"/>
@@ -328,14 +328,14 @@
     <t>Last Event Time</t>
   </si>
   <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>Puff/Inj Criteria
 &gt;3 mL: Inj
 &lt;2 mL: Puff
 &gt;2.5 mL/s: Inj
 &lt;2 mL/s: Puff</t>
+  </si>
+  <si>
+    <t>Duration (Minutes)</t>
   </si>
 </sst>
 </file>
@@ -924,10 +924,10 @@
   </sheetPr>
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="AO5" sqref="AO5"/>
+      <selection pane="bottomLeft" activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1071,7 @@
         <v>34</v>
       </c>
       <c r="AK1" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AL1" s="22" t="s">
         <v>36</v>
@@ -1080,7 +1080,7 @@
         <v>37</v>
       </c>
       <c r="AN1" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
       <c r="AL2" s="23"/>
       <c r="AM2" s="23"/>
       <c r="AN2" s="26">
-        <f>IF(AM2&gt;=AL2, (AM2-AL2)*1440, (AM2-AL2+1440)*1440)</f>
+        <f>IF(AM2&gt;=AL2, (AM2-AL2)*1440, (AM2-AL2+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       <c r="AL3" s="23"/>
       <c r="AM3" s="23"/>
       <c r="AN3" s="26">
-        <f t="shared" ref="AN3:AN66" si="11">IF(AM3&gt;=AL3, (AM3-AL3)*1440, (AM3-AL3+1440)*1440)</f>
+        <f t="shared" ref="AN3:AN66" si="11">IF(AM3&gt;=AL3, (AM3-AL3)*1440, (AM3-AL3+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -6161,7 +6161,7 @@
       <c r="AL67" s="23"/>
       <c r="AM67" s="23"/>
       <c r="AN67" s="26">
-        <f t="shared" ref="AN67:AN130" si="23">IF(AM67&gt;=AL67, (AM67-AL67)*1440, (AM67-AL67+1440)*1440)</f>
+        <f t="shared" ref="AN67:AN130" si="23">IF(AM67&gt;=AL67, (AM67-AL67)*1440, (AM67-AL67+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -11089,7 +11089,7 @@
       <c r="AL131" s="23"/>
       <c r="AM131" s="23"/>
       <c r="AN131" s="26">
-        <f t="shared" ref="AN131:AN194" si="35">IF(AM131&gt;=AL131, (AM131-AL131)*1440, (AM131-AL131+1440)*1440)</f>
+        <f t="shared" ref="AN131:AN194" si="35">IF(AM131&gt;=AL131, (AM131-AL131)*1440, (AM131-AL131+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -16017,7 +16017,7 @@
       <c r="AL195" s="23"/>
       <c r="AM195" s="23"/>
       <c r="AN195" s="26">
-        <f t="shared" ref="AN195:AN258" si="47">IF(AM195&gt;=AL195, (AM195-AL195)*1440, (AM195-AL195+1440)*1440)</f>
+        <f t="shared" ref="AN195:AN258" si="47">IF(AM195&gt;=AL195, (AM195-AL195)*1440, (AM195-AL195+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -20945,7 +20945,7 @@
       <c r="AL259" s="23"/>
       <c r="AM259" s="23"/>
       <c r="AN259" s="26">
-        <f t="shared" ref="AN259:AN322" si="59">IF(AM259&gt;=AL259, (AM259-AL259)*1440, (AM259-AL259+1440)*1440)</f>
+        <f t="shared" ref="AN259:AN322" si="59">IF(AM259&gt;=AL259, (AM259-AL259)*1440, (AM259-AL259+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -25873,7 +25873,7 @@
       <c r="AL323" s="23"/>
       <c r="AM323" s="23"/>
       <c r="AN323" s="26">
-        <f t="shared" ref="AN323:AN386" si="71">IF(AM323&gt;=AL323, (AM323-AL323)*1440, (AM323-AL323+1440)*1440)</f>
+        <f t="shared" ref="AN323:AN386" si="71">IF(AM323&gt;=AL323, (AM323-AL323)*1440, (AM323-AL323+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -30801,7 +30801,7 @@
       <c r="AL387" s="23"/>
       <c r="AM387" s="23"/>
       <c r="AN387" s="26">
-        <f t="shared" ref="AN387:AN450" si="83">IF(AM387&gt;=AL387, (AM387-AL387)*1440, (AM387-AL387+1440)*1440)</f>
+        <f t="shared" ref="AN387:AN450" si="83">IF(AM387&gt;=AL387, (AM387-AL387)*1440, (AM387-AL387+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -35729,7 +35729,7 @@
       <c r="AL451" s="23"/>
       <c r="AM451" s="23"/>
       <c r="AN451" s="26">
-        <f t="shared" ref="AN451:AN514" si="95">IF(AM451&gt;=AL451, (AM451-AL451)*1440, (AM451-AL451+1440)*1440)</f>
+        <f t="shared" ref="AN451:AN514" si="95">IF(AM451&gt;=AL451, (AM451-AL451)*1440, (AM451-AL451+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -40657,7 +40657,7 @@
       <c r="AL515" s="23"/>
       <c r="AM515" s="23"/>
       <c r="AN515" s="26">
-        <f t="shared" ref="AN515:AN578" si="107">IF(AM515&gt;=AL515, (AM515-AL515)*1440, (AM515-AL515+1440)*1440)</f>
+        <f t="shared" ref="AN515:AN578" si="107">IF(AM515&gt;=AL515, (AM515-AL515)*1440, (AM515-AL515+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -45585,7 +45585,7 @@
       <c r="AL579" s="23"/>
       <c r="AM579" s="23"/>
       <c r="AN579" s="26">
-        <f t="shared" ref="AN579:AN642" si="119">IF(AM579&gt;=AL579, (AM579-AL579)*1440, (AM579-AL579+1440)*1440)</f>
+        <f t="shared" ref="AN579:AN642" si="119">IF(AM579&gt;=AL579, (AM579-AL579)*1440, (AM579-AL579+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -50513,7 +50513,7 @@
       <c r="AL643" s="23"/>
       <c r="AM643" s="23"/>
       <c r="AN643" s="26">
-        <f t="shared" ref="AN643:AN706" si="131">IF(AM643&gt;=AL643, (AM643-AL643)*1440, (AM643-AL643+1440)*1440)</f>
+        <f t="shared" ref="AN643:AN706" si="131">IF(AM643&gt;=AL643, (AM643-AL643)*1440, (AM643-AL643+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -55441,7 +55441,7 @@
       <c r="AL707" s="23"/>
       <c r="AM707" s="23"/>
       <c r="AN707" s="26">
-        <f t="shared" ref="AN707:AN770" si="143">IF(AM707&gt;=AL707, (AM707-AL707)*1440, (AM707-AL707+1440)*1440)</f>
+        <f t="shared" ref="AN707:AN770" si="143">IF(AM707&gt;=AL707, (AM707-AL707)*1440, (AM707-AL707+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -60369,7 +60369,7 @@
       <c r="AL771" s="23"/>
       <c r="AM771" s="23"/>
       <c r="AN771" s="26">
-        <f t="shared" ref="AN771:AN834" si="155">IF(AM771&gt;=AL771, (AM771-AL771)*1440, (AM771-AL771+1440)*1440)</f>
+        <f t="shared" ref="AN771:AN834" si="155">IF(AM771&gt;=AL771, (AM771-AL771)*1440, (AM771-AL771+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -65297,7 +65297,7 @@
       <c r="AL835" s="23"/>
       <c r="AM835" s="23"/>
       <c r="AN835" s="26">
-        <f t="shared" ref="AN835:AN898" si="167">IF(AM835&gt;=AL835, (AM835-AL835)*1440, (AM835-AL835+1440)*1440)</f>
+        <f t="shared" ref="AN835:AN898" si="167">IF(AM835&gt;=AL835, (AM835-AL835)*1440, (AM835-AL835+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -70225,7 +70225,7 @@
       <c r="AL899" s="23"/>
       <c r="AM899" s="23"/>
       <c r="AN899" s="26">
-        <f t="shared" ref="AN899:AN962" si="179">IF(AM899&gt;=AL899, (AM899-AL899)*1440, (AM899-AL899+1440)*1440)</f>
+        <f t="shared" ref="AN899:AN962" si="179">IF(AM899&gt;=AL899, (AM899-AL899)*1440, (AM899-AL899+1)*1440)</f>
         <v>0</v>
       </c>
     </row>
@@ -75153,7 +75153,7 @@
       <c r="AL963" s="23"/>
       <c r="AM963" s="23"/>
       <c r="AN963" s="26">
-        <f t="shared" ref="AN963:AN1000" si="191">IF(AM963&gt;=AL963, (AM963-AL963)*1440, (AM963-AL963+1440)*1440)</f>
+        <f t="shared" ref="AN963:AN1000" si="191">IF(AM963&gt;=AL963, (AM963-AL963)*1440, (AM963-AL963+1)*1440)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>